<commit_message>
Scrum and Final Release Documentation updated/added to repo
</commit_message>
<xml_diff>
--- a/Scrum Documents/Sprint 1/Sprint 1 Burnup.xlsx
+++ b/Scrum Documents/Sprint 1/Sprint 1 Burnup.xlsx
@@ -76,7 +76,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr/>
+              <a:defRPr b="0"/>
             </a:pPr>
             <a:r>
               <a:t>Sprint 1 Burnup</a:t>
@@ -149,11 +149,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1189659044"/>
-        <c:axId val="1542616942"/>
+        <c:axId val="1290690350"/>
+        <c:axId val="1896382858"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1189659044"/>
+        <c:axId val="1290690350"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -164,14 +164,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr/>
+              <a:defRPr b="0"/>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1542616942"/>
+        <c:crossAx val="1896382858"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1542616942"/>
+        <c:axId val="1896382858"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -198,11 +198,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr/>
+              <a:defRPr b="0"/>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1189659044"/>
+        <c:crossAx val="1290690350"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>